<commit_message>
Definitely final cleanup lmao
</commit_message>
<xml_diff>
--- a/altium/build/BOM/Bill of Materials-Skayboard.xlsx
+++ b/altium/build/BOM/Bill of Materials-Skayboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\Skayboard\altium\build\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B412DE7-E8C6-4087-B372-E544CD49EB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E650FEB2-CAE7-4366-8F03-B50EF5055571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="10140" windowHeight="4740" xr2:uid="{C497C3A0-F6E9-4CB8-A424-BE2D9C193CBD}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="10140" windowHeight="4740" xr2:uid="{436B74E0-A0CE-4D50-97A8-A6252215DBCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Skayboard" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3004955A-39A7-48CD-A08F-F9F179A4B065}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22E0E10-CC80-4EED-9F46-6F66E66AB08B}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>